<commit_message>
fix: resolve #2 - Fixing DM Profile switching by modifing post condition
</commit_message>
<xml_diff>
--- a/Config/ChromeProfiles.xlsx
+++ b/Config/ChromeProfiles.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TwitterGrok 2.0\Twitter-RPA-Outreach-Bot\Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC90A3A-D520-43CD-8FDD-3B1FBC7F3C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Profile</t>
   </si>
@@ -28,13 +34,19 @@
   </si>
   <si>
     <t>Profile 4</t>
+  </si>
+  <si>
+    <t>Profile 1</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,34 +355,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: resolve #3 adding Restore tabs widnow popup handling mechanisim in diffrent stages
</commit_message>
<xml_diff>
--- a/Config/ChromeProfiles.xlsx
+++ b/Config/ChromeProfiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TwitterGrok 2.0\Twitter-RPA-Outreach-Bot\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC90A3A-D520-43CD-8FDD-3B1FBC7F3C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC55DE60-5E95-4194-B47F-7A1418BA8056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Profile</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>Profile 4</t>
-  </si>
-  <si>
-    <t>Profile 1</t>
-  </si>
-  <si>
-    <t>Default</t>
   </si>
 </sst>
 </file>
@@ -363,32 +357,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>